<commit_message>
Q3 2022 Fiscal Data update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BIR-Collection-Goals.xlsx
+++ b/Data/Fiscal Data/BIR-Collection-Goals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/236e6b124acc9753/Documents/Indicators/Data/Fiscal Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A282871-5F17-4709-ACD0-32C1AF6136F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C62422F-A0F8-4BC2-856A-51174F90F963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="3420" windowWidth="13305" windowHeight="8895" xr2:uid="{7A3B8417-BD7A-4E49-9332-F56347C45CB5}"/>
+    <workbookView xWindow="10890" yWindow="2985" windowWidth="13380" windowHeight="11385" xr2:uid="{7A3B8417-BD7A-4E49-9332-F56347C45CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="143">
   <si>
     <t>RMO</t>
   </si>
@@ -434,6 +434,36 @@
   </si>
   <si>
     <t>2021</t>
+  </si>
+  <si>
+    <t>RMO No. 27-2021</t>
+  </si>
+  <si>
+    <t>October 25, 2021</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202021/RMO%20No.%2027-2021_Annexes.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 16-2022</t>
+  </si>
+  <si>
+    <t>March 15, 2022</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO16-2022_Annexes.pdf</t>
+  </si>
+  <si>
+    <t>June 9, 2022</t>
+  </si>
+  <si>
+    <t>RMO No. 30-2022</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO%2030/RMO%20No.%2030-2022%20Table%205A-F.pdf</t>
   </si>
 </sst>
 </file>
@@ -793,12 +823,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFAD674-096D-4872-AE17-B99246C78A86}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,6 +1993,112 @@
       </c>
       <c r="K33" s="2">
         <v>181565</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="2">
+        <v>2081161</v>
+      </c>
+      <c r="G34" s="2">
+        <f>1015431+39712</f>
+        <v>1055143</v>
+      </c>
+      <c r="H34" s="2">
+        <v>305218</v>
+      </c>
+      <c r="I34" s="2">
+        <v>378721</v>
+      </c>
+      <c r="J34" s="2">
+        <v>127860</v>
+      </c>
+      <c r="K34" s="2">
+        <v>214219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="2">
+        <v>2438302</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1225218.0830000001</v>
+      </c>
+      <c r="H35" s="2">
+        <v>348345</v>
+      </c>
+      <c r="I35" s="2">
+        <v>501631.55300000001</v>
+      </c>
+      <c r="J35" s="2">
+        <v>136741.364</v>
+      </c>
+      <c r="K35" s="2">
+        <v>226366</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="2">
+        <v>2438302</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1225218.0830000001</v>
+      </c>
+      <c r="H36" s="2">
+        <v>348345</v>
+      </c>
+      <c r="I36" s="2">
+        <v>501631.55300000001</v>
+      </c>
+      <c r="J36" s="2">
+        <v>136741.364</v>
+      </c>
+      <c r="K36" s="2">
+        <v>226366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Q4 2022 Fiscal Data update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BIR-Collection-Goals.xlsx
+++ b/Data/Fiscal Data/BIR-Collection-Goals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Fiscal Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C62422F-A0F8-4BC2-856A-51174F90F963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E799ACD0-4C2D-496C-B270-877CB97E6ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10890" yWindow="2985" windowWidth="13380" windowHeight="11385" xr2:uid="{7A3B8417-BD7A-4E49-9332-F56347C45CB5}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{7A3B8417-BD7A-4E49-9332-F56347C45CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
   <si>
     <t>RMO</t>
   </si>
@@ -464,6 +464,15 @@
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO%2030/RMO%20No.%2030-2022%20Table%205A-F.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 53-2022</t>
+  </si>
+  <si>
+    <t>December 7, 2022</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Full%20Text/Revised%20CY2022%20RMO%20Goal%20Annexes.pdf</t>
   </si>
 </sst>
 </file>
@@ -823,12 +832,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFAD674-096D-4872-AE17-B99246C78A86}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,6 +2108,41 @@
       </c>
       <c r="K36" s="2">
         <v>226366</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="2">
+        <v>2392587</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1197966</v>
+      </c>
+      <c r="H37" s="2">
+        <v>365197</v>
+      </c>
+      <c r="I37" s="2">
+        <v>430160.55300000001</v>
+      </c>
+      <c r="J37" s="2">
+        <v>153695.364</v>
+      </c>
+      <c r="K37" s="2">
+        <v>245568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Q4 2022 Fiscal Data update"
This reverts commit 3a4ff00e04b845eca7d34efd64df7c17574852ac.
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BIR-Collection-Goals.xlsx
+++ b/Data/Fiscal Data/BIR-Collection-Goals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Fiscal Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E799ACD0-4C2D-496C-B270-877CB97E6ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C62422F-A0F8-4BC2-856A-51174F90F963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{7A3B8417-BD7A-4E49-9332-F56347C45CB5}"/>
+    <workbookView xWindow="10890" yWindow="2985" windowWidth="13380" windowHeight="11385" xr2:uid="{7A3B8417-BD7A-4E49-9332-F56347C45CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="143">
   <si>
     <t>RMO</t>
   </si>
@@ -464,15 +464,6 @@
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO%2030/RMO%20No.%2030-2022%20Table%205A-F.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 53-2022</t>
-  </si>
-  <si>
-    <t>December 7, 2022</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Full%20Text/Revised%20CY2022%20RMO%20Goal%20Annexes.pdf</t>
   </si>
 </sst>
 </file>
@@ -832,12 +823,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFAD674-096D-4872-AE17-B99246C78A86}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,41 +2099,6 @@
       </c>
       <c r="K36" s="2">
         <v>226366</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>145</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="2">
-        <v>2392587</v>
-      </c>
-      <c r="G37" s="2">
-        <v>1197966</v>
-      </c>
-      <c r="H37" s="2">
-        <v>365197</v>
-      </c>
-      <c r="I37" s="2">
-        <v>430160.55300000001</v>
-      </c>
-      <c r="J37" s="2">
-        <v>153695.364</v>
-      </c>
-      <c r="K37" s="2">
-        <v>245568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Q4 2022 Fiscal Data update""
This reverts commit 1008de8ab618a2b40aed746c17ff1cb3dcd72cec.
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BIR-Collection-Goals.xlsx
+++ b/Data/Fiscal Data/BIR-Collection-Goals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Fiscal Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Fiscal Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C62422F-A0F8-4BC2-856A-51174F90F963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E799ACD0-4C2D-496C-B270-877CB97E6ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10890" yWindow="2985" windowWidth="13380" windowHeight="11385" xr2:uid="{7A3B8417-BD7A-4E49-9332-F56347C45CB5}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{7A3B8417-BD7A-4E49-9332-F56347C45CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
   <si>
     <t>RMO</t>
   </si>
@@ -464,6 +464,15 @@
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO%2030/RMO%20No.%2030-2022%20Table%205A-F.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 53-2022</t>
+  </si>
+  <si>
+    <t>December 7, 2022</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Full%20Text/Revised%20CY2022%20RMO%20Goal%20Annexes.pdf</t>
   </si>
 </sst>
 </file>
@@ -823,12 +832,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFAD674-096D-4872-AE17-B99246C78A86}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,6 +2108,41 @@
       </c>
       <c r="K36" s="2">
         <v>226366</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="2">
+        <v>2392587</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1197966</v>
+      </c>
+      <c r="H37" s="2">
+        <v>365197</v>
+      </c>
+      <c r="I37" s="2">
+        <v>430160.55300000001</v>
+      </c>
+      <c r="J37" s="2">
+        <v>153695.364</v>
+      </c>
+      <c r="K37" s="2">
+        <v>245568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Q3 2023 Fiscal Data Update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BIR-Collection-Goals.xlsx
+++ b/Data/Fiscal Data/BIR-Collection-Goals.xlsx
@@ -1,58 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Fiscal Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E799ACD0-4C2D-496C-B270-877CB97E6ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{7A3B8417-BD7A-4E49-9332-F56347C45CB5}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+  <si>
+    <t>Link</t>
+  </si>
   <si>
     <t>RMO</t>
   </si>
   <si>
+    <t>IssueDate</t>
+  </si>
+  <si>
+    <t>TargetCY</t>
+  </si>
+  <si>
     <t>Version</t>
   </si>
   <si>
-    <t>IssueDate</t>
-  </si>
-  <si>
-    <t>RMO No. 11-2002</t>
-  </si>
-  <si>
-    <t>May 10, 2002</t>
-  </si>
-  <si>
-    <t>TargetCY</t>
+    <t>Goal_TotalRevenue</t>
+  </si>
+  <si>
+    <t>Goal_NetIncomeandProfits</t>
+  </si>
+  <si>
+    <t>Goal_ExciseTaxes</t>
+  </si>
+  <si>
+    <t>Goal_ValueAddedTaxes</t>
+  </si>
+  <si>
+    <t>Goal_PercentageTaxes</t>
+  </si>
+  <si>
+    <t>Goal_OtherTaxes</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/9637rmo11_tables%201-9.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 11-2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 10, 2002</t>
   </si>
   <si>
     <t>2002</t>
@@ -61,76 +64,52 @@
     <t>Initial</t>
   </si>
   <si>
-    <t>RMO No. 26-2002</t>
-  </si>
-  <si>
-    <t>October 9, 2002</t>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/4216rmo26_tbls.%201-9.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 26-2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 9, 2002</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/2357rmo03_20.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 20-2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 4, 2003</t>
   </si>
   <si>
     <t>2003</t>
   </si>
   <si>
-    <t>Final</t>
-  </si>
-  <si>
-    <t>Goal_TotalRevenue</t>
-  </si>
-  <si>
-    <t>Goal_NetIncomeandProfits</t>
-  </si>
-  <si>
-    <t>Goal_ExciseTaxes</t>
-  </si>
-  <si>
-    <t>Goal_ValueAddedTaxes</t>
-  </si>
-  <si>
-    <t>Goal_PercentageTaxes</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/9637rmo11_tables%201-9.pdf</t>
-  </si>
-  <si>
-    <t>Goal_OtherTaxes</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/4216rmo26_tbls.%201-9.pdf</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/2357rmo03_20.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 20-2003</t>
-  </si>
-  <si>
-    <t>June 4, 2003</t>
-  </si>
-  <si>
     <t>Initial/Final</t>
   </si>
   <si>
-    <t>RMO No. 6-2004</t>
-  </si>
-  <si>
-    <t>February 17, 2004</t>
-  </si>
-  <si>
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/1798rmo04_06tab1.pdf</t>
   </si>
   <si>
+    <t xml:space="preserve">RMO No. 6-2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 17, 2004</t>
+  </si>
+  <si>
     <t>2004</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/15713rmo05-02%20(tables).pdf</t>
   </si>
   <si>
-    <t>RMO No. 2-2005</t>
-  </si>
-  <si>
-    <t>January 18, 2005</t>
+    <t xml:space="preserve">RMO No. 2-2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 18, 2005</t>
   </si>
   <si>
     <t>2005</t>
@@ -139,10 +118,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/28330rmo06_06tables.pdf</t>
   </si>
   <si>
-    <t>RMO No. 6-2006</t>
-  </si>
-  <si>
-    <t>February 15, 2006</t>
+    <t xml:space="preserve">RMO No. 6-2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 15, 2006</t>
   </si>
   <si>
     <t>2006</t>
@@ -151,10 +130,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/34743Tables.pdf</t>
   </si>
   <si>
-    <t>RMO No. 7-2007</t>
-  </si>
-  <si>
-    <t>April 27, 2007</t>
+    <t xml:space="preserve">RMO No. 7-2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 27, 2007</t>
   </si>
   <si>
     <t>2007</t>
@@ -163,10 +142,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/39979RMO%2017-2008%20Annexes.pdf</t>
   </si>
   <si>
-    <t>RMO No. 17-2008</t>
-  </si>
-  <si>
-    <t>May 16, 2008</t>
+    <t xml:space="preserve">RMO No. 17-2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 16, 2008</t>
   </si>
   <si>
     <t>2008</t>
@@ -175,10 +154,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/45613Annexes_rmo7-09.pdf</t>
   </si>
   <si>
-    <t>RMO No. 7-2009</t>
-  </si>
-  <si>
-    <t>April 6 , 2009</t>
+    <t xml:space="preserve">RMO No. 7-2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 6 , 2009</t>
   </si>
   <si>
     <t>2009</t>
@@ -187,310 +166,333 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/46675amended%20annexes%20of%20rmo%2025.PDF</t>
   </si>
   <si>
-    <t>RMO No. 25-2009</t>
-  </si>
-  <si>
-    <t>July 9, 2009</t>
-  </si>
-  <si>
-    <t>RMO No. 31-2010</t>
-  </si>
-  <si>
-    <t>March 24, 2010</t>
+    <t xml:space="preserve">RMO No. 25-2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 9, 2009</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/50100Annexes_rmo_31-2010_revised_again.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 31-2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 24, 2010</t>
   </si>
   <si>
     <t>2010</t>
   </si>
   <si>
-    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/50100Annexes_rmo_31-2010_revised_again.pdf</t>
-  </si>
-  <si>
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/52599RMO%2066-2010-Annexes.pdf</t>
   </si>
   <si>
-    <t>RMO No. 66-2010</t>
-  </si>
-  <si>
-    <t>July 30, 2010</t>
+    <t xml:space="preserve">RMO No. 66-2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 30, 2010</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/57045ANNEXES_for%20email.pdf</t>
   </si>
   <si>
-    <t>RMO No. 12-2011</t>
-  </si>
-  <si>
-    <t>March 17, 2011</t>
+    <t xml:space="preserve">RMO No. 12-2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 17, 2011</t>
   </si>
   <si>
     <t>2011</t>
   </si>
   <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/61827Copy%20of%20ANNEXES_RMO1-2012.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 1-2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 12, 2012</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/68142Table1.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 1-2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 24, 2013</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/81226Tables%20RMO%204-2014.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 4-2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 16, 2014</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/81819Tables%20RMO%207-2014.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 7-2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 24, 2014</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%202%20Table%201.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 2-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 13, 2015</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%204%20Annexes%20Table%201%20to%205.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 4-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 6, 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revision 1</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%20No.%205-2015%20Annexes%20Table%201%20to%205.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 5-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 12, 2015</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202016/RMO%20No.%202-2016%20Annexes%20Table%201%20to%205.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 2-2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 8, 2016</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202017/RMO%207%20-%202017%20Tables.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 7-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 16, 2017</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202018/Tables%201-4%20and%205A-5F.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 8-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 29, 2018</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202018/Tables%201-4%20and%205A-5F_copy.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 10-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 22, 2018</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/RMO%209-2019/RMO%209-2019%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 9-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 11, 2019</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/Revised%20CY%202019%20BIR%20Goal_Tables%202-5F.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 18-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 26, 2019</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/RMO%2029-2019%20Tables%202-5F.PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 29-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 6, 2019</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%202-2020%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 2-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 16, 2020</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%20No.%2012-2020%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 12-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 27, 2020</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%20Annexes_pdf.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 16-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 16, 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revision 2</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/Annexes_pdf.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 30-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 22, 2020</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202021/RMO_No.%207-2021_Annexes_CY%202021%20GOAL.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 7-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2, 2021</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202021/RMO%20No.%2027-2021_Annexes.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 27-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 25, 2021</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO16-2022_Annexes.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 16-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 15, 2022</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO%2030/RMO%20No.%2030-2022%20Table%205A-F.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 30-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 9, 2022</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Full%20Text/Revised%20CY2022%20RMO%20Goal%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 53-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 7, 2022</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2023/Full%20Text/CY2023_RMO%20Annexes_based%20on%20MTRP%20Dec.5%202022-BL.PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 15-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 25, 2023</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2023/RMO%20No.%2027-2023/Revised_CY2023_RMO%20Annexes%201.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 27-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 27, 2023</t>
+  </si>
+  <si>
+    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2023/RMO%20No.%2034-2023/RMO%20No.%2034-2023%20Table%202%20to%205F.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMO No. 34-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 19, 2023</t>
+  </si>
+  <si>
     <t>https://www.bir.gov.ph/index.php/revenue-issuances/revenue-memorandum-orders/rmo-py.html</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/61827Copy%20of%20ANNEXES_RMO1-2012.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 1-2012</t>
-  </si>
-  <si>
-    <t>January 12, 2012</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/68142Table1.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 1-2013</t>
-  </si>
-  <si>
-    <t>January 24, 2013</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/81226Tables%20RMO%204-2014.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 4-2014</t>
-  </si>
-  <si>
-    <t>January 16, 2014</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/81819Tables%20RMO%207-2014.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 7-2014</t>
-  </si>
-  <si>
-    <t>January 24, 2014</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%202%20Table%201.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 2-2015</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>January 13, 2015</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%204%20Annexes%20Table%201%20to%205.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 4-2015</t>
-  </si>
-  <si>
-    <t>February 6, 2015</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%20No.%205-2015%20Annexes%20Table%201%20to%205.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 5-2015</t>
-  </si>
-  <si>
-    <t>March 12, 2015</t>
-  </si>
-  <si>
-    <t>Revision 1</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202016/RMO%20No.%202-2016%20Annexes%20Table%201%20to%205.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 2-2016</t>
-  </si>
-  <si>
-    <t>January 8, 2016</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202017/RMO%207%20-%202017%20Tables.xlsx</t>
-  </si>
-  <si>
-    <t>RMO No. 7-2017</t>
-  </si>
-  <si>
-    <t>March 16, 2017</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202018/Tables%201-4%20and%205A-5F.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 8-2018</t>
-  </si>
-  <si>
-    <t>January 29, 2018</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202018/Tables%201-4%20and%205A-5F_copy.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 10-2018</t>
-  </si>
-  <si>
-    <t>February 22, 2018</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/RMO%209-2019/RMO%209-2019%20Annexes.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 9-2019</t>
-  </si>
-  <si>
-    <t>February 11, 2019</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/Revised%20CY%202019%20BIR%20Goal_Tables%202-5F.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 18-2019</t>
-  </si>
-  <si>
-    <t>April 26, 2019</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/RMO%2029-2019%20Tables%202-5F.PDF</t>
-  </si>
-  <si>
-    <t>RMO No. 29-2019</t>
-  </si>
-  <si>
-    <t>June 6, 2019</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%202-2020%20Annexes.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 2-2020</t>
-  </si>
-  <si>
-    <t>January 16, 2020</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%20No.%2012-2020%20Annexes.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 12-2020</t>
-  </si>
-  <si>
-    <t>April 27, 2020</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%20Annexes_pdf.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 16-2020</t>
-  </si>
-  <si>
-    <t>June 16, 2020</t>
-  </si>
-  <si>
-    <t>Revision 2</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/Annexes_pdf.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 30-2020</t>
-  </si>
-  <si>
-    <t>September 22, 2020</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202021/RMO_No.%207-2021_Annexes_CY%202021%20GOAL.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 7-2021</t>
-  </si>
-  <si>
-    <t>February 2, 2021</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>RMO No. 27-2021</t>
-  </si>
-  <si>
-    <t>October 25, 2021</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202021/RMO%20No.%2027-2021_Annexes.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 16-2022</t>
-  </si>
-  <si>
-    <t>March 15, 2022</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO16-2022_Annexes.pdf</t>
-  </si>
-  <si>
-    <t>June 9, 2022</t>
-  </si>
-  <si>
-    <t>RMO No. 30-2022</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO%2030/RMO%20No.%2030-2022%20Table%205A-F.pdf</t>
-  </si>
-  <si>
-    <t>RMO No. 53-2022</t>
-  </si>
-  <si>
-    <t>December 7, 2022</t>
-  </si>
-  <si>
-    <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Full%20Text/Revised%20CY2022%20RMO%20Goal%20Annexes.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -504,20 +506,21 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="4">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,15 +531,295 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -578,108 +861,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -687,7 +876,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -713,7 +902,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -765,16 +954,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -790,7 +991,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -821,84 +1022,76 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFAD674-096D-4872-AE17-B99246C78A86}">
-  <dimension ref="A1:K37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="3" width="17.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="2" customWidth="1"/>
-    <col min="7" max="11" width="12.85546875" style="2"/>
+    <col customWidth="1" min="2" max="3" style="1" width="17.140625"/>
+    <col customWidth="1" min="4" max="4" style="1" width="10.7109375"/>
+    <col customWidth="1" min="5" max="5" style="1" width="12.85546875"/>
+    <col customWidth="1" min="6" max="6" style="2" width="10.7109375"/>
+    <col min="7" max="11" style="2" width="12.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="F2" s="2">
         <v>447556</v>
@@ -919,21 +1112,21 @@
         <v>24105</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2">
         <v>422516</v>
@@ -954,18 +1147,18 @@
         <v>26810</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
@@ -989,15 +1182,15 @@
         <v>22307</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>28</v>
@@ -1024,7 +1217,7 @@
         <v>31081</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1059,7 +1252,7 @@
         <v>29355</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1094,7 +1287,7 @@
         <v>31528</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1129,7 +1322,7 @@
         <v>43684</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1164,7 +1357,7 @@
         <v>53652</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1178,7 +1371,7 @@
         <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F10" s="2">
         <v>865572</v>
@@ -1199,7 +1392,7 @@
         <v>56908</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1213,7 +1406,7 @@
         <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F11" s="2">
         <v>798455</v>
@@ -1234,21 +1427,21 @@
         <v>56504</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F12" s="2">
         <v>830441</v>
@@ -1269,7 +1462,7 @@
         <v>52786</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1280,10 +1473,10 @@
         <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F13" s="2">
         <v>860441</v>
@@ -1304,7 +1497,7 @@
         <v>46754</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1339,18 +1532,18 @@
         <v>55491</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
@@ -1374,18 +1567,18 @@
         <v>61242</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" t="s">
         <v>69</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
@@ -1409,21 +1602,21 @@
         <v>62762</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" t="s">
         <v>73</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F17" s="2">
         <v>1456330</v>
@@ -1444,21 +1637,21 @@
         <v>78240</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" t="s">
         <v>77</v>
       </c>
-      <c r="C18" t="s">
-        <v>78</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F18" s="2">
         <v>1425297</v>
@@ -1479,21 +1672,21 @@
         <v>73221</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F19" s="2">
         <v>1720846</v>
@@ -1514,21 +1707,21 @@
         <v>86958</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F20" s="2">
         <v>1703946</v>
@@ -1549,7 +1742,7 @@
         <v>86958</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -1563,7 +1756,7 @@
         <v>81</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F21" s="2">
         <v>1673946</v>
@@ -1584,18 +1777,18 @@
         <v>86958</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
@@ -1619,18 +1812,18 @@
         <v>123536</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
@@ -1642,33 +1835,33 @@
         <v>1099740.8999999999</v>
       </c>
       <c r="H23" s="2">
-        <v>185028.6</v>
+        <v>185028.60000000001</v>
       </c>
       <c r="I23" s="2">
-        <v>364431.3</v>
+        <v>364431.29999999999</v>
       </c>
       <c r="J23" s="2">
-        <v>73346.2</v>
+        <v>73346.199999999997</v>
       </c>
       <c r="K23" s="2">
         <v>106701.5</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F24" s="2">
         <v>2039152</v>
@@ -1689,21 +1882,21 @@
         <v>137950.908</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F25" s="2">
         <v>2039152</v>
@@ -1724,21 +1917,21 @@
         <v>137753.908</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F26" s="2">
         <v>2330693</v>
@@ -1759,21 +1952,21 @@
         <v>189125</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F27" s="2">
         <v>2271373</v>
@@ -1794,21 +1987,21 @@
         <v>227036</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F28" s="2">
         <v>2330693</v>
@@ -1829,21 +2022,21 @@
         <v>189125</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F29" s="2">
         <v>2576003</v>
@@ -1864,21 +2057,21 @@
         <v>225399</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="D30" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F30" s="2">
         <v>2260484</v>
@@ -1899,21 +2092,21 @@
         <v>183314</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="F31" s="2">
         <v>1744104</v>
@@ -1934,21 +2127,21 @@
         <v>143579</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32">
       <c r="A32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F32" s="2">
         <v>1685734</v>
@@ -1969,21 +2162,21 @@
         <v>143432</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33">
       <c r="A33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F33" s="2">
         <v>2081161</v>
@@ -2004,9 +2197,9 @@
         <v>181565</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>133</v>
@@ -2015,10 +2208,10 @@
         <v>134</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F34" s="2">
         <v>2081161</v>
@@ -2040,9 +2233,9 @@
         <v>214219</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>136</v>
@@ -2054,7 +2247,7 @@
         <v>138</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F35" s="2">
         <v>2438302</v>
@@ -2075,21 +2268,21 @@
         <v>226366</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F36" s="2">
         <v>2438302</v>
@@ -2110,9 +2303,9 @@
         <v>226366</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37">
       <c r="A37" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>143</v>
@@ -2124,7 +2317,7 @@
         <v>138</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F37" s="2">
         <v>2392587</v>
@@ -2145,27 +2338,140 @@
         <v>245568</v>
       </c>
     </row>
+    <row r="38" ht="14.25">
+      <c r="A38" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="2">
+        <v>2599127</v>
+      </c>
+      <c r="G38" s="2">
+        <v>1368921</v>
+      </c>
+      <c r="H38" s="2">
+        <v>352876</v>
+      </c>
+      <c r="I38" s="2">
+        <v>507027</v>
+      </c>
+      <c r="J38" s="2">
+        <v>125049</v>
+      </c>
+      <c r="K38" s="2">
+        <f>230480+14774</f>
+        <v>245254</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F39" s="2">
+        <v>2639174</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1397523</v>
+      </c>
+      <c r="H39" s="2">
+        <v>336093</v>
+      </c>
+      <c r="I39" s="2">
+        <v>538131</v>
+      </c>
+      <c r="J39" s="2">
+        <v>124646</v>
+      </c>
+      <c r="K39" s="2">
+        <v>242781</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="2">
+        <v>2639174</v>
+      </c>
+      <c r="G40" s="2">
+        <f>1316452+81071</f>
+        <v>1397523</v>
+      </c>
+      <c r="H40" s="2">
+        <v>336093</v>
+      </c>
+      <c r="I40" s="2">
+        <v>538131</v>
+      </c>
+      <c r="J40" s="2">
+        <v>124646</v>
+      </c>
+      <c r="K40" s="2">
+        <f>224154+18627</f>
+        <v>242781</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B6A2EE-F788-4EC7-8DB4-876B3AA7B8B1}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q2 2024 Fiscal Data update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/BIR-Collection-Goals.xlsx
+++ b/Data/Fiscal Data/BIR-Collection-Goals.xlsx
@@ -1,20 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Fiscal Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE80379-2C47-48C5-A1BB-4FBF100B1AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="3225" yWindow="4515" windowWidth="11145" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="163">
   <si>
     <t>Link</t>
   </si>
@@ -52,10 +72,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/9637rmo11_tables%201-9.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 11-2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 10, 2002</t>
+    <t>RMO No. 11-2002</t>
+  </si>
+  <si>
+    <t>May 10, 2002</t>
   </si>
   <si>
     <t>2002</t>
@@ -67,10 +87,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/4216rmo26_tbls.%201-9.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 26-2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 9, 2002</t>
+    <t>RMO No. 26-2002</t>
+  </si>
+  <si>
+    <t>October 9, 2002</t>
   </si>
   <si>
     <t>Final</t>
@@ -79,10 +99,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/2357rmo03_20.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 20-2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 4, 2003</t>
+    <t>RMO No. 20-2003</t>
+  </si>
+  <si>
+    <t>June 4, 2003</t>
   </si>
   <si>
     <t>2003</t>
@@ -94,10 +114,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/1798rmo04_06tab1.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 6-2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 17, 2004</t>
+    <t>RMO No. 6-2004</t>
+  </si>
+  <si>
+    <t>February 17, 2004</t>
   </si>
   <si>
     <t>2004</t>
@@ -106,10 +126,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/15713rmo05-02%20(tables).pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 2-2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 18, 2005</t>
+    <t>RMO No. 2-2005</t>
+  </si>
+  <si>
+    <t>January 18, 2005</t>
   </si>
   <si>
     <t>2005</t>
@@ -118,10 +138,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/28330rmo06_06tables.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 6-2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 15, 2006</t>
+    <t>RMO No. 6-2006</t>
+  </si>
+  <si>
+    <t>February 15, 2006</t>
   </si>
   <si>
     <t>2006</t>
@@ -130,10 +150,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/34743Tables.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 7-2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 27, 2007</t>
+    <t>RMO No. 7-2007</t>
+  </si>
+  <si>
+    <t>April 27, 2007</t>
   </si>
   <si>
     <t>2007</t>
@@ -142,10 +162,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/39979RMO%2017-2008%20Annexes.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 17-2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May 16, 2008</t>
+    <t>RMO No. 17-2008</t>
+  </si>
+  <si>
+    <t>May 16, 2008</t>
   </si>
   <si>
     <t>2008</t>
@@ -154,10 +174,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/45613Annexes_rmo7-09.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 7-2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 6 , 2009</t>
+    <t>RMO No. 7-2009</t>
+  </si>
+  <si>
+    <t>April 6 , 2009</t>
   </si>
   <si>
     <t>2009</t>
@@ -166,19 +186,19 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/46675amended%20annexes%20of%20rmo%2025.PDF</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 25-2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 9, 2009</t>
+    <t>RMO No. 25-2009</t>
+  </si>
+  <si>
+    <t>July 9, 2009</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/50100Annexes_rmo_31-2010_revised_again.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 31-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 24, 2010</t>
+    <t>RMO No. 31-2010</t>
+  </si>
+  <si>
+    <t>March 24, 2010</t>
   </si>
   <si>
     <t>2010</t>
@@ -187,19 +207,19 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/52599RMO%2066-2010-Annexes.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 66-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 30, 2010</t>
+    <t>RMO No. 66-2010</t>
+  </si>
+  <si>
+    <t>July 30, 2010</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/57045ANNEXES_for%20email.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 12-2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 17, 2011</t>
+    <t>RMO No. 12-2011</t>
+  </si>
+  <si>
+    <t>March 17, 2011</t>
   </si>
   <si>
     <t>2011</t>
@@ -208,10 +228,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/61827Copy%20of%20ANNEXES_RMO1-2012.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 1-2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 12, 2012</t>
+    <t>RMO No. 1-2012</t>
+  </si>
+  <si>
+    <t>January 12, 2012</t>
   </si>
   <si>
     <t>2012</t>
@@ -220,10 +240,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/68142Table1.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 1-2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 24, 2013</t>
+    <t>RMO No. 1-2013</t>
+  </si>
+  <si>
+    <t>January 24, 2013</t>
   </si>
   <si>
     <t>2013</t>
@@ -232,10 +252,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/81226Tables%20RMO%204-2014.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 4-2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 16, 2014</t>
+    <t>RMO No. 4-2014</t>
+  </si>
+  <si>
+    <t>January 16, 2014</t>
   </si>
   <si>
     <t>2014</t>
@@ -244,19 +264,19 @@
     <t>https://www.bir.gov.ph/images/bir_files/old_files/pdf/81819Tables%20RMO%207-2014.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 7-2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 24, 2014</t>
+    <t>RMO No. 7-2014</t>
+  </si>
+  <si>
+    <t>January 24, 2014</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%202%20Table%201.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 2-2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 13, 2015</t>
+    <t>RMO No. 2-2015</t>
+  </si>
+  <si>
+    <t>January 13, 2015</t>
   </si>
   <si>
     <t>2015</t>
@@ -265,31 +285,31 @@
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%204%20Annexes%20Table%201%20to%205.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 4-2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 6, 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revision 1</t>
+    <t>RMO No. 4-2015</t>
+  </si>
+  <si>
+    <t>February 6, 2015</t>
+  </si>
+  <si>
+    <t>Revision 1</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202015/RMO%20No.%205-2015%20Annexes%20Table%201%20to%205.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 5-2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 12, 2015</t>
+    <t>RMO No. 5-2015</t>
+  </si>
+  <si>
+    <t>March 12, 2015</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Full%20Text%20of%20RMO%202016/RMO%20No.%202-2016%20Annexes%20Table%201%20to%205.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 2-2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 8, 2016</t>
+    <t>RMO No. 2-2016</t>
+  </si>
+  <si>
+    <t>January 8, 2016</t>
   </si>
   <si>
     <t>2016</t>
@@ -298,10 +318,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202017/RMO%207%20-%202017%20Tables.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 7-2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 16, 2017</t>
+    <t>RMO No. 7-2017</t>
+  </si>
+  <si>
+    <t>March 16, 2017</t>
   </si>
   <si>
     <t>2017</t>
@@ -310,10 +330,10 @@
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202018/Tables%201-4%20and%205A-5F.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 8-2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 29, 2018</t>
+    <t>RMO No. 8-2018</t>
+  </si>
+  <si>
+    <t>January 29, 2018</t>
   </si>
   <si>
     <t>2018</t>
@@ -322,19 +342,19 @@
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202018/Tables%201-4%20and%205A-5F_copy.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 10-2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 22, 2018</t>
+    <t>RMO No. 10-2018</t>
+  </si>
+  <si>
+    <t>February 22, 2018</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/RMO%209-2019/RMO%209-2019%20Annexes.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 9-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 11, 2019</t>
+    <t>RMO No. 9-2019</t>
+  </si>
+  <si>
+    <t>February 11, 2019</t>
   </si>
   <si>
     <t>2019</t>
@@ -343,28 +363,28 @@
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/Revised%20CY%202019%20BIR%20Goal_Tables%202-5F.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 18-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 26, 2019</t>
+    <t>RMO No. 18-2019</t>
+  </si>
+  <si>
+    <t>April 26, 2019</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202019/RMO%2029-2019%20Tables%202-5F.PDF</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 29-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 6, 2019</t>
+    <t>RMO No. 29-2019</t>
+  </si>
+  <si>
+    <t>June 6, 2019</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%202-2020%20Annexes.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 2-2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">January 16, 2020</t>
+    <t>RMO No. 2-2020</t>
+  </si>
+  <si>
+    <t>January 16, 2020</t>
   </si>
   <si>
     <t>2020</t>
@@ -373,40 +393,40 @@
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%20No.%2012-2020%20Annexes.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 12-2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 27, 2020</t>
+    <t>RMO No. 12-2020</t>
+  </si>
+  <si>
+    <t>April 27, 2020</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/RMO%20Annexes_pdf.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 16-2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 16, 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revision 2</t>
+    <t>RMO No. 16-2020</t>
+  </si>
+  <si>
+    <t>June 16, 2020</t>
+  </si>
+  <si>
+    <t>Revision 2</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202020/Annexes_pdf.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 30-2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September 22, 2020</t>
+    <t>RMO No. 30-2020</t>
+  </si>
+  <si>
+    <t>September 22, 2020</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202021/RMO_No.%207-2021_Annexes_CY%202021%20GOAL.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 7-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February 2, 2021</t>
+    <t>RMO No. 7-2021</t>
+  </si>
+  <si>
+    <t>February 2, 2021</t>
   </si>
   <si>
     <t>2021</t>
@@ -415,19 +435,19 @@
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/Attachments%20of%20RMO%202021/RMO%20No.%2027-2021_Annexes.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 27-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 25, 2021</t>
+    <t>RMO No. 27-2021</t>
+  </si>
+  <si>
+    <t>October 25, 2021</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO16-2022_Annexes.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 16-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March 15, 2022</t>
+    <t>RMO No. 16-2022</t>
+  </si>
+  <si>
+    <t>March 15, 2022</t>
   </si>
   <si>
     <t>2022</t>
@@ -436,28 +456,28 @@
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Attachments/RMO%2030/RMO%20No.%2030-2022%20Table%205A-F.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 30-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June 9, 2022</t>
+    <t>RMO No. 30-2022</t>
+  </si>
+  <si>
+    <t>June 9, 2022</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2022/Full%20Text/Revised%20CY2022%20RMO%20Goal%20Annexes.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 53-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December 7, 2022</t>
+    <t>RMO No. 53-2022</t>
+  </si>
+  <si>
+    <t>December 7, 2022</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2023/Full%20Text/CY2023_RMO%20Annexes_based%20on%20MTRP%20Dec.5%202022-BL.PDF</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 15-2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April 25, 2023</t>
+    <t>RMO No. 15-2023</t>
+  </si>
+  <si>
+    <t>April 25, 2023</t>
   </si>
   <si>
     <t>2023</t>
@@ -466,31 +486,52 @@
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2023/RMO%20No.%2027-2023/Revised_CY2023_RMO%20Annexes%201.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 27-2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 27, 2023</t>
+    <t>RMO No. 27-2023</t>
+  </si>
+  <si>
+    <t>July 27, 2023</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/images/bir_files/internal_communications_3/2023/RMO%20No.%2034-2023/RMO%20No.%2034-2023%20Table%202%20to%205F.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">RMO No. 34-2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October 19, 2023</t>
+    <t>RMO No. 34-2023</t>
+  </si>
+  <si>
+    <t>October 19, 2023</t>
   </si>
   <si>
     <t>https://www.bir.gov.ph/index.php/revenue-issuances/revenue-memorandum-orders/rmo-py.html</t>
+  </si>
+  <si>
+    <t>RMO No. 11-2024</t>
+  </si>
+  <si>
+    <t>March 14, 2024</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/RMO%20No.%2011-2024%20Annexes.pdf</t>
+  </si>
+  <si>
+    <t>RMO No. 29-2024</t>
+  </si>
+  <si>
+    <t>July 22, 2024</t>
+  </si>
+  <si>
+    <t>https://bir-cdn.bir.gov.ph/BIR/pdf/CY2024%20Goal%20_RMO%2029-2024%20Annexes.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -506,21 +547,20 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,295 +571,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1022,27 +782,30 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection activeCell="A38" sqref="A38"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="3" style="1" width="17.140625"/>
-    <col customWidth="1" min="4" max="4" style="1" width="10.7109375"/>
-    <col customWidth="1" min="5" max="5" style="1" width="12.85546875"/>
-    <col customWidth="1" min="6" max="6" style="2" width="10.7109375"/>
-    <col min="7" max="11" style="2" width="12.85546875"/>
+    <col min="2" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="7" max="11" width="12.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1112,7 +875,7 @@
         <v>24105</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1147,7 +910,7 @@
         <v>26810</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1182,7 +945,7 @@
         <v>22307</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1217,7 +980,7 @@
         <v>31081</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1252,7 +1015,7 @@
         <v>29355</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1287,7 +1050,7 @@
         <v>31528</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1322,7 +1085,7 @@
         <v>43684</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1357,7 +1120,7 @@
         <v>53652</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1392,7 +1155,7 @@
         <v>56908</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1427,7 +1190,7 @@
         <v>56504</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1462,7 +1225,7 @@
         <v>52786</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1497,7 +1260,7 @@
         <v>46754</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1532,7 +1295,7 @@
         <v>55491</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1567,7 +1330,7 @@
         <v>61242</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1602,7 +1365,7 @@
         <v>62762</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1637,7 +1400,7 @@
         <v>78240</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -1672,7 +1435,7 @@
         <v>73221</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1707,7 +1470,7 @@
         <v>86958</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -1742,7 +1505,7 @@
         <v>86958</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -1777,7 +1540,7 @@
         <v>86958</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -1812,7 +1575,7 @@
         <v>123536</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1835,19 +1598,19 @@
         <v>1099740.8999999999</v>
       </c>
       <c r="H23" s="2">
-        <v>185028.60000000001</v>
+        <v>185028.6</v>
       </c>
       <c r="I23" s="2">
-        <v>364431.29999999999</v>
+        <v>364431.3</v>
       </c>
       <c r="J23" s="2">
-        <v>73346.199999999997</v>
+        <v>73346.2</v>
       </c>
       <c r="K23" s="2">
         <v>106701.5</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -1882,7 +1645,7 @@
         <v>137950.908</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>101</v>
       </c>
@@ -1917,7 +1680,7 @@
         <v>137753.908</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -1952,7 +1715,7 @@
         <v>189125</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>108</v>
       </c>
@@ -1987,7 +1750,7 @@
         <v>227036</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -2022,7 +1785,7 @@
         <v>189125</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2057,7 +1820,7 @@
         <v>225399</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -2092,7 +1855,7 @@
         <v>183314</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>121</v>
       </c>
@@ -2127,7 +1890,7 @@
         <v>143579</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -2162,7 +1925,7 @@
         <v>143432</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -2197,7 +1960,7 @@
         <v>181565</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -2233,7 +1996,7 @@
         <v>214219</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>135</v>
       </c>
@@ -2268,7 +2031,7 @@
         <v>226366</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -2303,7 +2066,7 @@
         <v>226366</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -2338,20 +2101,20 @@
         <v>245568</v>
       </c>
     </row>
-    <row r="38" ht="14.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>145</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F38" s="2">
@@ -2374,20 +2137,20 @@
         <v>245254</v>
       </c>
     </row>
-    <row r="39" ht="14.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>149</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F39" s="2">
@@ -2409,7 +2172,7 @@
         <v>242781</v>
       </c>
     </row>
-    <row r="40" ht="14.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -2419,10 +2182,10 @@
       <c r="C40" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F40" s="2">
@@ -2446,32 +2209,101 @@
         <v>242781</v>
       </c>
     </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="2">
+        <v>3055169</v>
+      </c>
+      <c r="G41" s="2">
+        <f>1649267+72127</f>
+        <v>1721394</v>
+      </c>
+      <c r="H41" s="2">
+        <v>326195</v>
+      </c>
+      <c r="I41" s="2">
+        <v>599235</v>
+      </c>
+      <c r="J41" s="2">
+        <v>163216</v>
+      </c>
+      <c r="K41" s="2">
+        <f>229242+15887</f>
+        <v>245129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="2">
+        <v>3046751.2749999999</v>
+      </c>
+      <c r="G42" s="2">
+        <f>1467398.307+ 85227.022</f>
+        <v>1552625.3289999999</v>
+      </c>
+      <c r="H42" s="2">
+        <v>457812.31400000001</v>
+      </c>
+      <c r="I42" s="2">
+        <v>620708.23899999994</v>
+      </c>
+      <c r="J42" s="2">
+        <v>144379.228</v>
+      </c>
+      <c r="K42" s="2">
+        <f>255339.165+ 15887</f>
+        <v>271226.16500000004</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>155</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>